<commit_message>
Get daily reddit data: Tue Jan  9 08:08:24 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_01_14.xlsx
+++ b/data/2024_01_14.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C459"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,2692 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1929m1s</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Early for Valentine's but I love the colors</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/opf9kywsfdbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1928z8g</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Cow nails!!! 🐮</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9iv4665b8dbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>19277h3</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Clear (ish) shellac</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z1pnscbbpcbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>19275bk</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>I'm Sorry my friend has a bad habbit😬😅</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cbndny8pocbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1926qzd</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>My nails for January</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1926qzd</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>19249uf</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Recommended regular/non-gel polishes and techniques for velvet nails?</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19249uf/recommended_regularnongel_polishes_and_techniques/</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1924m9b</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Clase Azul or Corningware? 😂</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8y3dfdwi1cbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1924bk6</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>I got this set done yesterday, and today the pinky nail came off.</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8tfrbujxybbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>19249oo</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>just a monthly gel x pic</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mxgdugqiybbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1924851</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Opinions on nail refills?</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1924851/opinions_on_nail_refills/</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>19247mi</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Help with Gel-X air bubbles?</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h0aqylr3ybbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1923y3x</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Gel doesn’t last</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1923y3x</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1923mlt</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Custom press ons</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1923mlt/custom_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1921y4j</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Video and pics don’t do these nails justice 🥺</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/z9zzgxw4fbbc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1921ggp</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Barbie pink marble nails (first time doing marble!)</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oki56146bbbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>19211nq</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Spirited Away!</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19211nq</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1920v97</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Paddie Polygel Nails</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1920v97/paddie_polygel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>191zq39</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Love this blue 🥰</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/djgqg4amxabc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>191z9i7</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Is soaking feet in high temperature water with mustard soap or apple cider vinegar before a pedicure a good idea?</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/191z9i7/is_soaking_feet_in_high_temperature_water_with/</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>191z0ae</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>First time getting BIAB nails! 🎀</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/191z0ae</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>191yw3z</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Do you like spicy cateye? I did my nails for a back-to-uni confidence boost (◍´ᯅ `◍)</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/191yw3z</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>191ypgn</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Feeling the blue fantasy today &amp; created these 🦋</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/191ypgn</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>191ylpl</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Plain or painted</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/191ylpl</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>191yjjq</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Are acrylic nails bad for you</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/191yjjq/are_acrylic_nails_bad_for_you/</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>191xun5</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>In love with this set ❤️</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a0r44dbujabc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>191wxn3</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Any naruto fans here? 3D Orochimaru set for my client, hand painted and sculpted by me 🐍</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jvybo7ccdabc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>191wp7w</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Hand painted lace frenchies</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/191wp7w</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>191wed2</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Advise needed - biab keeps separating from nail</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/191wed2</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>191w6rz</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>First set of 2024!</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/191w6rz</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>191w2lc</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>What do you think? feedback is appreciated 🖤</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/191w2lc</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>191vwnm</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Been a minute</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4d3a0mx26abc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>191vvpi</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>3d aurora chrome nails</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/191vvpi</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>191vuyw</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Rubber base bends</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ipmf10vs5abc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>191vjjx</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Black French Tips 😍</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/so8rwzvg3abc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>191v973</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>second time drawing (not bad ig)</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bts4db9e1abc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>191v8fj</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>nails in what style do you like them?</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ueys67h81abc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>191v2cc</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>My first time with baby boomer :) I LOVE IT</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/191v2cc</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>191utpl</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Neutral color polishes browning?</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/191utpl/neutral_color_polishes_browning/</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>191uswp</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Some work from our family owned and operated salon</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/191uswp</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>191uo1g</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Soft green pedi</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/191uo1g</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>191ukjj</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Im obsessed 😍</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bx4n4vekw9bc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>191u9fc</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Halp. I thought I was a lifer with my acrylics but I’m looking for an alternative. Totally lost</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jxc3m16iu9bc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>191tm8q</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Just had my nails done</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a20mnxivp9bc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>191sx13</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>What kind of manicure did I get?</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/191sx13/what_kind_of_manicure_did_i_get/</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>191su5m</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Anyone a Lovecraft Fan? I made some Shoggoth nails to boost my confidence for first day of new college term.. The eyes glow too</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xk3kf2dfk9bc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>191sikp</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>My nails look horrible. They won't grow, break for no reason, middle left nail splits down the middle. Any suggestions? Please.</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3bc7tlw0i9bc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>191rerd</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>New nails</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/191rerd</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>191qrzq</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Nails breaking under dip powder?</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/191qrzq</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>191sa3p</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Gel nail is coming off. Short time remedies?</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zmntwx9bg9bc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>191ppv3</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>do my nails look unhealthy ? i have iron deficiency anaemia and that causes me to have weak nails that break easily</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qd4vtp8yx8bc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>191rmhs</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>New Year Nails⭐️</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jpkb1uzjb9bc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>191rkf7</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>New set I did, what do you think?</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/191rkf7</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>191rb8w</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>I use to HATE rounded/almond shaped nails. Now look at me😂</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/191rb8w</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>191qtvm</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Goodbye Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xl8p0wwz59bc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>191qa4a</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>January Snowflakes</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ztmgnw329bc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>191q94d</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>French Nails - Personally, loved this set. Would love to know what the sub feels ! :)</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8gyapqqw19bc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>191pzi8</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>French tips</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/191pzi8</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>191pxje</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>snowflake!</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/191pxje</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>191pcw6</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Aurora powder</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tge4dm08v8bc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>191p7qo</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>How to (very politely) fire my nail tech?</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/191p7qo/how_to_very_politely_fire_my_nail_tech/</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>191ov0z</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Thoughts?</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bbpg5j7ir8bc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>191osg0</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Nails I just did! Nothing revolutionary and kinda messy but I've literally never done nail art so I'm pretty proud :)</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/191osg0</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>191kfu3</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>My nails really stress when they get long</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vfkg1xmvp7bc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>191o3pr</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>What stands up best to water?</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/191o3pr/what_stands_up_best_to_water/</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>191nxs1</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Obsessed is an understatement 💙</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2x3i9s5fk8bc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>191nnmx</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Japanese hard gel ♥️</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sqkcj105i8bc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>191ncai</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Recent nails</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/usywo0njf8bc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>191mvfk</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>So proud of My Wife!</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/191mvfk</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>191mnvn</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Bomb sales!</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://dtknailsupply.com/collections/dnd-dc-nail-lacquer</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>191mnva</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Almond or coffin?</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/191mnva</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>191llqy</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Would love any cc 🥰</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/191llqy</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>191l6gw</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Okay ladies need some insight on nail printers.</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/191l6gw/okay_ladies_need_some_insight_on_nail_printers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>191kuhw</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Natural beauty</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/191kuhw</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>191kc5l</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>My new bright and shiny nails</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/191kc5l</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>191k7or</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Doing my mom's nails as a beginner 🫶🏻</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/asneqxugn7bc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>191k2bj</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Rabbit strawberry design I got done last month. My nails grew so strong since then</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zbt9ulsvl7bc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>191jwjj</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Tried a new color today</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v7y6c1t6k7bc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>191jnu9</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>Before I say goodbye to them - my holiday nails this year ✨🦌</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/74lf66dkh7bc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>191i205</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>My 1st time getting my nails done</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/symo82ybz6bc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>191htkk</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>missing this set i did last summer 😩❤️</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/191htkk</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>191gzqc</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>I’m 16, I’ve been doing nails since august. This is the first “client” I’ve ever had, how’d I do?</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jsjsrmr7m6bc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>191d84g</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Can my chrome nails be fixed?☹️</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/191d84g</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>191g7cf</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Second try! It's a lot better this time. the shapes are kind of inconsistent, but besides that any criticism?</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/191g7cf</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1929gu7</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Where to buy nail polish in Spain (Madrid &amp; Barcelona) and Portugal?</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1929gu7/where_to_buy_nail_polish_in_spain_madrid/</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1926gc7</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>The most mesmerizing polish ever</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lcfryofxhcbc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1926fte</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Super Duper proud of my collection, finally finished swatches</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b8b42ilshcbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>19257gx</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Finally achieved the dream!</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19257gx</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>19253hq</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Lamenting fall 🍂🦀</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ulxpy7zn5cbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1924lo1</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Another Zoya 10 for $25 Haul (with swatches)</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1924lo1</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>192292g</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>What I do instead of buying things:</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192292g</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1924fg0</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Pinkish red recommendations</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1924fg0/pinkish_red_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>192496r</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Is it just me or are these completely different colors?</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ej8a7yxeybbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1923ooj</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Cracks in polish?</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1923ooj/cracks_in_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1923mxq</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Any suggestions for (preferably shimmery) polishes roughly in this shade of bluish green?</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1923mxq</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1922zka</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Matte Black + Rose Magnetic Polish</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fqzuuqrrnbbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1922jpo</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>So satisfying</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1922jpo</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1922cir</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>‘Elsa-from-frozen’ mani</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8undzftgibbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>19222la</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Cuticula Mic Drop discontinued?</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19222la/cuticula_mic_drop_discontinued/</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1921u56</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Do we have any physicists here that can explain magnets?</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1921u56</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1921hz5</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Oldies but goodies</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1921hz5</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1920tut</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>My office always has the best lighting</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1920tut</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>191zr93</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Sad to say Goodbye to Holiday Lights. Happy to say Hello to Holo Lights.</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8js8r2vuxabc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>191zf79</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>My collection 🤍</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/191zf79</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>191z5tn</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>KB shimmer ring magnet</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/191z5tn/kb_shimmer_ring_magnet/</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>191z54a</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Dip dupe for gel OPI Tiramisu for Two?</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/191z54a/dip_dupe_for_gel_opi_tiramisu_for_two/</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>191z1ld</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Would the heart magnet trend work for us?</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/40ewmhfhsabc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>191yx0e</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Wake up ! and Don’t Resist! 💜💗💙</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7ahg9fjkrabc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>191yxm3</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>BKL mystery bag reveal 🦄💦</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/191yxm3</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>191ycrj</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>It’s BOROmir not STEALmir</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gur0bkgjnabc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>191xwz4</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Need to vent about the nail tech that I'm never seeing again</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/191xwz4/need_to_vent_about_the_nail_tech_that_im_never/</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>191xcif</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Baby's first Holo</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://imgur.com/gallery/3c69GGU</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>191x854</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Went short, on one hand. Swipe for broken nail</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/LE20URH</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>191vmxc</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Snowstorm inspired ❄️</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jq14pqm54abc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>191v2tg</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Mardi Gras mani!</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/m8ksnwz40abc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>191v1u8</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>One of My Favorite Polishes of All Time: BKL Unmade</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/191v1u8</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>191uxi3</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Funny thing is I was proud of my nails today</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dsfhngh3z9bc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>191urfq</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Does anyone know of a good dupe for this color? Maybe shades that are a bit darker and/or more champagne?</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/191urfq</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>191uly0</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Went from rarely wearing green to it being a favorite 🍃💚🌿</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/191uly0</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>191t332</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>I like these, but feel like they need a gem placement. Where would you put it?</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/191t332</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>191ss2c</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>What nail polishes to use for these looks?</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/191ss2c</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>191s1pl</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Home is Where my Butt is by Wildflower Lacquer</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/191s1pl</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>191sem8</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Alchemy Lacquers Parrot Waxcap 😍</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/191sem8</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>191s4qo</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Mega (S) by ILNP</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/191s4qo</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>191s4qn</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Sprinkles!</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3hsswxn7f9bc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>191rrlp</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>practicing french tips 😅</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kfq0645lc9bc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>191qsun</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Why does my nail look like this even with piling/buttering?</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ddc6k2fs59bc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>191pvgs</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Finally nailed magnetics!</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/191pvgs</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>191pr7n</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>First Snow ❄️</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/191pr7n</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>191pi3m</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>matcha cloud</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/191pi3m</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>191pg7v</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Mermaid bait mani</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/191pg7v</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>191p5l9</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>May regret later but pulled the trigger on celebratory gel nails while in Korea!</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/191p5l9</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>191p1gz</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>First mani</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mxvhqw5us8bc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>191oyf2</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Wondering why I can't get Opi Infinite Shine to look good</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/191oyf2/wondering_why_i_cant_get_opi_infinite_shine_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>191otm0</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Holo Taco Advice?</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a8km6fk7r8bc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>191oovo</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>My nails are too short to show off the dark blue thermal! Orly bonder, Prism Polish - Freezing My Baguettes Off, Seche Vite</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n5vd0lrxp8bc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>191mjww</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Convincing yourself you don't need new polish...we've all been there, right?</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/19h8npix88bc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>191o9qh</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Another sexy shifter from ILNP</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/191o9qh</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>191o8wf</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>There’s snow on the ground, but clovers on my nails ☘️</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/191o8wf</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>191nzn4</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>The snow gods haven't been in a giving mood this season... Until this weekend 😁🥰</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6k5d0a3uk8bc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>191nysc</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Question about flakes used in polishes: chameleon, aurora, multichrome, iridescent...can anyone help clarify the differences?</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/191nysc/question_about_flakes_used_in_polishes_chameleon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>191nyc4</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Obsessed is an understatement 💙</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5b26xknjk8bc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>191m3a1</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>When you have the best coworkers ever...</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zsdaxknz48bc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>191kqvf</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>I need a thinner antidote</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/191kqvf/i_need_a_thinner_antidote/</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>191k0pv</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>First time using a thermal polish!</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vbzw6qxel7bc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>191iphs</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/191iphs/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>191hd1z</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Feeling Blue-tiful Today &lt;3</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qsaifm3rq6bc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>191gvwg</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Grandmas &amp; Nail Polish</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u7qikeowk6bc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1929exs</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Any Recommendations for Nail Salons in Granville?</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1929exs/any_recommendations_for_nail_salons_in_granville/</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1928jlg</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Set I just did.</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/acpjf5cc3dbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>19237qx</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Simple but my love!!!</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oup0vqzyobbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>19213j2</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>What do we think?</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19213j2</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>191wo3k</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>I think this might be my favorite set 🧸</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2dk4n0rgbabc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>191utb5</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Soft green pedi set</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/191utb5</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>191o7bc</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>Goodbye Christmas Nails!!</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/goig5kzhm8bc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>191nfxj</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>Colourful start of the year 🎨✨</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/191nfxj</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>191ms17</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>My Wife is Amazing</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/191ms17</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>191kzf9</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Winter nails</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v59hzdx0v7bc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>191i5ii</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Cyberpunk press ons 👽💚</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wfs67uvg07bc1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Jan 10 08:08:24 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_01_14.xlsx
+++ b/data/2024_01_14.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C459"/>
+  <dimension ref="A1:C621"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8236,6 +8236,2760 @@
         </is>
       </c>
     </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>19334dj</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Late Xmas Winter Nails</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19334dj</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1932bnq</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>black and white french</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p13zmmmpakbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1931vyb</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>(first post) dream nails for the winter season ✨🫧❄️🤍</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/glzoy7gq5kbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>193176k</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Fave nails I've done on myself ❤️</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0rdd051myjbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1930xup</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Natural Nails ❌ Reinforcement Gel</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ek570x0wjbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>192zyzy</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>My nails are horrible!</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/77ooxndsmjbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>192zai7</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>My current set of false nails I made (products below)</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f1uv2z9igjbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>192z2aq</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Pink cow nails! How did I do?</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192z2aq</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>192z1aq</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Jade Nails</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192z1aq</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>192w0n0</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>UPDATE on my thick, teeth like nails: new manicure done by jojonailsslc</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192w0n0</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>192xh3r</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>New to diy builder gel fill</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192xh3r</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>192x4ff</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Bday Gift For my Girlfriend</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/192x4ff/bday_gift_for_my_girlfriend/</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>192x1b8</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Acrylic removal</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/192x1b8/acrylic_removal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>192wwff</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>Back to Square (Round?) One 🥲</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192wwff</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>192w8cb</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Soft gel</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ivea1g0apibc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>192w45c</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Baby blue sparkly french 💙</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192w45c</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>192vae8</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>first time getting gel x !</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192vae8</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>192v9z2</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>Almost 3 weeks since last fill - that aside, why do these look so “off”</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192v9z2</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>192v87n</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>This is my 4th time doing my own nails, if you’re a nail tech can you tell me how I’m doing?</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4kv1b7c3hibc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>192urmd</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>13th Birthday colors.</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192urmd</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>192uqzq</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Fresh Out 🌸</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j7lga3a1dibc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>192tr7s</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>Galaxy 🌌 Nail Set</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kstap3pn5ibc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>192tnra</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Summer nails</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192tnra</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>192ti6n</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>worth $85 + $10 tip?</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pgqqkufq3ibc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>192r0as</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Does anyone know of a dupe?</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192r0as</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>192rgys</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>how do i ask for nails like this? (credit @nails_by_annabel_m on IG)</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mr6iejj0phbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>192t50z</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>Green glitter 💚</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bkcll2h11ibc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>192sfto</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Help! How to preserve my nails at the beach</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/192sfto/help_how_to_preserve_my_nails_at_the_beach/</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>192s9vk</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>Simple Frenchie with a dash of glitz✨</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rfcqs7osuhbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>192ob99</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>Snakes! I love this one so much! It was so much fun!</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192ob99</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>192o36b</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>What do you all do when your non-natural nails pop off or break?</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/192o36b/what_do_you_all_do_when_your_nonnatural_nails_pop/</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>192n9yy</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>some nail growth plus a bagel</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192n9yy</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>192mq7g</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Icy pastels for this chilly January 🥶</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192mq7g</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>192mgei</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>My nail tech ATEEE. Nails were art deco inspired.</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yx4myktfpgbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>192q126</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Basic natural nail mani</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192q126</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>192lcgg</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Why are my nails peeling even with regular polish?</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/192lcgg/why_are_my_nails_peeling_even_with_regular_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>192l0gh</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Why does my gel polish always do this?</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/imtnz923fgbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>192pmjh</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Dip powder combined with the gel on the toes? Or just gel?</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/192pmjh/dip_powder_combined_with_the_gel_on_the_toes_or/</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>192p4js</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>My pretty cool powerpuff girl(s) nails from this summer!</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/845hnpeb8hbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>192oviz</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>What nail glue do you guys use? I bought the KISS nail glue but keep getting dried out ones 🥲</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/192oviz/what_nail_glue_do_you_guys_use_i_bought_the_kiss/</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>192ouad</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Does this nail shape and length suit my long fingers?</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192ouad</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>192oqou</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>Tips</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/192oqou/tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>192o503</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>had a go at aura nails on gel x</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192o503</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>192o3tl</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>Bubble issues - advice, please!</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b4dx3p431hbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>192nzjv</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>I was so happy with how my nails were growing too 😭</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2yhl3d890hbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>192nvqp</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>First time doing gel nails!</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192nvqp</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>192nupz</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>Hey fellow nail art enthusiasts!</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yo8wcmz7zgbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>192nk84</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Live life in Armonía</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ljz2q3b8xgbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>192ni7s</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Do you think a square would suit me better? Need a change!</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192ni7s</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>192ngsy</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Poly gel set!</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192ngsy</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>192mirb</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>a bit early, but minimalist Valentine's Day theme</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/efjqqcqupgbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>192m5gn</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>advice for beginner</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/192m5gn/advice_for_beginner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>192m3fa</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Wearing gel nails for 4 weeks</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/192m3fa/wearing_gel_nails_for_4_weeks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>192lt4r</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>New set done with structure gel!</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7bh9cu1tkgbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>192lbxs</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Nail growth</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/192lbxs/nail_growth/</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>192l642</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>I have become completely obsessed with chrome</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/329mut08ggbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>192jqd5</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Blue and pink squiggly things</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192jqd5</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>192kpwm</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>Mirror, mirror....</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192kpwm</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>192khj3</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>It’s not easy being green 🐸💚🌈</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192khj3</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>192k548</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>butterfly nails i did yesterday!</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o6sl4rar8gbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>192jyh0</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Adventure time set I did! Opinions?</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bwhnq7ke7gbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>192jr81</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Rest in peace, soldier.</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i23gus1x5gbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>192jkbe</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Loving this holographic copper color on my shorties. EllaMilla in the color Enchanted</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/soxd7keo4gbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>192izo8</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>My new years nails</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/urm98tbl0gbc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>192i4jm</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Is The Gel Bottle worth it?</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/192i4jm/is_the_gel_bottle_worth_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>192i2j0</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Second set of gel nails that i have ever done and the first set i have done on myself 💙🩵</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/79mhfhmwtfbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>192i0jj</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Second Stamping</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192i0jj</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>192hu7q</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Poly nails?</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/192hu7q/poly_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>192hp09</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Any suggestions for design or colours if I want something buttery / honey/ pancake like</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/192hp09/any_suggestions_for_design_or_colours_if_i_want/</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>192hsno</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Simple French 💅</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3v1lb5kvrfbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>192d84i</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Regular Polish + good physical management is better than tech + nail polsih</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/192d84i/regular_polish_good_physical_management_is_better/</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>192hd06</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Recommendations?</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/192hd06/recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>192h89t</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>First time doing rose marble nails</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192h89t</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>192gssn</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Favourite cats eye gel?</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/192gssn/favourite_cats_eye_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>192gqsz</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Currently</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bxizolxijfbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>192g6pl</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>How can I improve the shape and look?</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192g6pl</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>192fvsj</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>New set!</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192fvsj</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>192fonk</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>As a massive Kirsty Meakin fan...the excitement is real! Eeeek!</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mod0brcrafbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>192fitn</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>french manicure with glitter</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rpd6iqtc9fbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>192fe7w</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>3 month Progress🥰</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192fe7w</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>192fa81</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>Red</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2449f69d7fbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>192eug2</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>how to get started out using gel-x?</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/192eug2/how_to_get_started_out_using_gelx/</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>192epur</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>I tried on some pretty nails from Tiktok!</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gabtc6ob2fbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>192eop7</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>Cirque Dream within a Dream</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/u2ophi302fbc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>192dm2t</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>marble nails~</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192dm2t</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>192dht1</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Been doing my own nails for a while now</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192dht1</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>192cxju</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>First gel polish</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/njautug8kebc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>192cwnr</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Same but different</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192cwnr</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>192b72r</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>silver chrome press ons</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192b72r</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1932e7f</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Help! Can I improve my nail pics or is my camera just 💩? (ILNP 'Juliette')</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1932e7f</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1931ohj</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Best shimmer toppers?</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1931ohj/best_shimmer_toppers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>192zr6o</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Mooncat Bottled Rage</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192zr6o</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>192zdhd</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Mooncat matte polish chipping?</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/192zdhd/mooncat_matte_polish_chipping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>192zcbg</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Spaceoddity by Mooncat</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192zcbg</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>192z75p</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Space saving organization?</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/192z75p/space_saving_organization/</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>192ybcd</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Which one of these Essies?</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/192ybcd/which_one_of_these_essies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>192y38n</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>I need a long lasting mani!!</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/192y38n/i_need_a_long_lasting_mani/</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>192xspp</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Polish Color for French Manicure</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gnuwss0q2jbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>192xa5i</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>My Xmas polishes arrived</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192xa5i</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>192x25d</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>Birthday Cake Nails</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192x25d</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>192wyuw</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>filing painted nails?</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/192wyuw/filing_painted_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>192wwya</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Playing around for St Pat’s</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nduk9zk4vibc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>192vlsu</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>mooncat mani!</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192vlsu</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>192udgf</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>Such a crisp and wintery color 🤤</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192udgf</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>192tz7l</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Just casually photographing my nails in the middle of a Costco</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192tz7l</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>192tnzp</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Final-ish Update! Nail Polish Cabinet custom build</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192tnzp</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>192q0o8</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Thermal Polish Lost its Mojo</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192q0o8</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>192tg0o</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Snowy twilight vibes</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7n4wdgqa3ibc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>192tewv</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>This topper just makes everything better 🩷🤍🩵</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uuhh9ty13ibc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>192sz0n</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Purple comparisons!</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192sz0n</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>192swd3</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Slick Slate</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192swd3</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>192sw2j</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Flakie Bomb</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192sw2j</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>192sp3n</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>ILNP - Fairy Dust</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192sp3n</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>192sfc1</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Crazy that this is the same color!</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192sfc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>192sezi</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Mooncat brush</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/192sezi/mooncat_brush/</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>192r1et</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Does essie contain formaldehyde?</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/192r1et/does_essie_contain_formaldehyde/</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>192qyg2</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Jelly opal nails ft. my cold red hands</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192qyg2</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>192qevl</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>unintentional Elsa mani</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vvop9z4hhhbc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>192qby6</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Does anyone own "Pluto" or "Goofy" from Nailtopia?</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tmwuvccxghbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>192pvvg</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>{PR} Misty by ILNP 💕</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dgkiyn4qdhbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>192psd7</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Snowy nails for a snowy day ❄️</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192psd7</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>192p9on</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Ethereal matte glow!</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tv0cz4069hbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>192p4b2</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>🍄</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mnovcjm98hbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>192nxuu</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>One Eyed One Horned Glowy Holo Purple Blue!!!</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192nxuu</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>192nsac</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>To teach us about our past</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192nsac</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>192ne7g</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Finally tried House of Hades</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192ne7g</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>192mmaa</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Valentines Sticker Mani!</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192mmaa</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>192meme</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>📺TV Test Pattern📺</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192meme</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>192m6xl</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Crackle Polish Topper</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192m6xl</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>192lsjb</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Cirque Velvetine 💜</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192lsjb</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>192loj8</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Seasonally inappropriate 🤨</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ic1zzlowjgbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>192kx6g</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Desperately looking for a dupe</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/192kx6g/desperately_looking_for_a_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>192ku3y</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>Indie polishes....❤💜</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192ku3y</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>192ktzp</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Lost Berry is so eye catching 💗🍓</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192ktzp</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>192jr0f</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Super bright claws for the new year!</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192jr0f</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>192jg3c</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Disney nails for Disney world!</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/df8i9p4v3gbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>192jbf9</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>ISO gel polish brands</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/192jbf9/iso_gel_polish_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>192ilno</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Ethereal's Dionysus — Such a lovely polish!</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192ilno</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>192ik3d</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>new year, new mani roundup + reviews!</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192ik3d</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>192ietx</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>This week’s mani (so far)</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aazbp21gwfbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>192hz9p</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Pretty Nice</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192hz9p</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>192gxus</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Favorite Periwinkle Shades?</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/192gxus/favorite_periwinkle_shades/</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>192g6g0</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Thank the nail gods with me that none of my nails broke while changing a tire</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192g6g0</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>192g2rv</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Color Club - Magic Attraction 🪩</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192g2rv</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>192fs0p</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>The shift is unreal ✨</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zotfzeqgbfbc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>192escz</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Another Blue Velvet Magnet Hack</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/a201hkwv2fbc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>192dsde</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>RIP</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192dsde</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>192bj9i</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Glass Jellyfish over jellies</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/na0bgh724ebc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>192bc0p</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>In love with Rue Morgue</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v31pdg0l1ebc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1931cwb</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>OMG, it's perfect for my short nails!</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1931cwb</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>192yz8n</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>My clients sets last week ✨</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192yz8n</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>192wxtw</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>I’ve been practicing my butterflies</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/igocezzbvibc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>192qkhq</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Nail Art by Trish at Cozy Nails in Madison, WI</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3v1346olihbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>192o6mm</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Cat eye Stripes</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/t2vi8uao1hbc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>192nuwv</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Te las harías??</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wk39ex1czgbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>192no89</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Try #2 painting gel nails to look like stones. These are inspired by white labradorite. I can't seem to capture the shift but there is an iridescent layer that peaks through in some spots. I hope you guys like them :)</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z8zq4yaqxgbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>192lzvo</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Strawberries &amp; Lace 🍓💗</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192lzvo</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>192lo7x</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Galactic 😊 first gel set of the year</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n8zyesgujgbc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>192ktfd</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>I just did these strawberry themed press-on nails.</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bi3kkzvpdgbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>192i2f8</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Round poly gel set</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192i2f8</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>192g2xd</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>My 5th attempt painting nails💗</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192g2xd</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>192f6mt</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>⛓️🩸🔗🔪👽🗡️ nails</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/192f6mt</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Jan 11 08:08:26 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_01_14.xlsx
+++ b/data/2024_01_14.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C621"/>
+  <dimension ref="A1:C808"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10990,6 +10990,3185 @@
         </is>
       </c>
     </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>193w9vc</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Recovered chronic nail biter</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193w9vc</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>193w9b2</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>First Gel X set</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193w9b2</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>193w4cq</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>does it look frozen?</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jhp9eb19lrbc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>193v6su</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>my current obsession is bows 🎀🩷</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6c7wk6mearbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>193unxv</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>First time buying press on. Is the apex meant to be this curved?</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193unxv</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>193uc5l</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Hard as Hoof</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/193uc5l/hard_as_hoof/</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>193uaku</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Some of my favorite nails so far! New into getting them done and having SO much fun with it!</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193uaku</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>193tw80</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>IBD hard gel as nail glue?</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/193tw80/ibd_hard_gel_as_nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>193tlja</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Got my nails done today with rubber base. Do they look well done?</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uvwzi32utqbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>193t6yf</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>What are some good polygel brands? What about drills?</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/193t6yf/what_are_some_good_polygel_brands_what_about/</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>193sgzc</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Are snowflake nails only for Christmas?</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/193sgzc/are_snowflake_nails_only_for_christmas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>193scty</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>First time ever doing my nails and I’m absolutely in love</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6w5qkvp6iqbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>193sag7</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Tried chrome powder on gel x for the first time ✨🪩</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wqhtmiwkhqbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>193s7qm</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>Can nail glue fix broken natural nails?</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/193s7qm/can_nail_glue_fix_broken_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>193s1ah</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>NYE Nails: Obsessed 😍</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hyv7t4x8fqbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>193p04g</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Hard gels</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/193p04g/hard_gels/</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>193nnai</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Best press on nails for clubbed thumb?</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193nnai</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>193m43s</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>How to get nails like these? Pictures from insta @peaknail</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193m43s</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>193rl1k</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Classy but slutty 💕</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f7zzoin5bqbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>193r8s7</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>still getting the hang of polygel</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193r8s7</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>193qhlp</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Valentine’s Day dip powder ideas? Preferably containing purple ?</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/193qhlp/valentines_day_dip_powder_ideas_preferably/</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>193qhdc</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Anyone else has sparkly green nails right now? 😁 Here are mine!</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pa7o52tk1qbc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>193q541</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Best gel dip liquids for DIY use?</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/193q541/best_gel_dip_liquids_for_diy_use/</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>193pqp3</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>gradient magnetic nails</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fntci0m9vpbc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>193p7aw</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Is this a good shape for me?</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6qz2l8hoqpbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>193p472</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>dewy butterfly nails🦋✨</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193p472</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>193ou7b</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Twinning with my baby</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ugveel2qnpbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>193o7pq</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Does this look Maryland themed? 🦀</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9zzh43ylipbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>193nm3m</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>How much do you think these sets cost?</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193nm3m</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>193mtve</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>Celestial nails for the new year ✨ Soft gel with chrome and charm accents on natural nails</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/go5x0fdo7pbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>193ms0k</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>NAILS FACING… UP?!!</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4uzmway97pbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>193mnba</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Does using Dip without activator change the color</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/193mnba/does_using_dip_without_activator_change_the_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>193mg4j</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Hammered Copper Nails</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6wiw1bgo4pbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>193mbw8</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>New setttt😍😍 my nail tech is amazing I appreciate her the most nails by @nailsbycin</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h1m5vpnq3pbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>193m68x</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Am I right to be disappointed?</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193m68x</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>193m08i</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Some simple goth stilettos this time.</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193m08i</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>193lry9</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>First try with Mizhse Cat Eye gel polishes.</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193lry9</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>193locm</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Made a post a week ago about playing guitar with longer nails</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/621guu9wyobc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>193lk21</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>Bare my soul - OPI</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193lk21</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>193lgl0</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>How to price out nail sets?? Help please!!</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193lgl0</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>193ko9g</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Stitch</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bdcgcxclrobc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>193jys2</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Can you help me figure out which nail shape suits me best please? Also can we appreciate my biab journey! I've gone from chronic biter to having nails!</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193jys2</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>193jgmq</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Any suggestions for nail design</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/193jgmq/any_suggestions_for_nail_design/</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>193im6t</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Cuticle advice please</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oqga0cdrcobc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>193ie0v</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Galaxy nails!</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193ie0v</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>193id09</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>First chrome nails</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dqnr4ymxaobc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>193i04e</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Tips for natural nails</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/193i04e/tips_for_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>193hplb</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Soft green mani set</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193hplb</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>193hlxy</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>base😍</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6uyaxpog5obc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>193hl4r</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>My artist absolutely killed it!</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193hl4r</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>193hik2</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>My Christmas gift to myself!</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/edxgspoy4obc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>193hfr3</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>I haven’t had shorties in ages!</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8z02n4ie4obc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>193hejs</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>First fresh set of the new year!</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3zsw6h654obc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>193h9bi</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>what do yall think of these ? never had this shape or color before but i think i like! i was going for a vintage look 🍒</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2mlkyzn13obc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>193gdo5</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Can you tell these are press on??</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193gdo5</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>193go5d</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>What do you think?</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193go5d</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>193ghb4</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Lumpy space princess vibes to start the new year 👑</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/e8lq6tfhxnbc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>193gajh</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Asked for rose gold chrome but I don’t mind this colour</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xyq36o83wnbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>193fokg</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>My current set I did :D</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193fokg</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>193fc5v</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Worth $64USD?</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c82lisk9pnbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>193f4j3</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Tried coffin nails for the first time</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cuzi93wqnnbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>193eeqh</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Extra wide press ons?</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/193eeqh/extra_wide_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>193ecmm</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>Apex</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/193ecmm/apex/</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>193dyvo</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>My first take on Coquette nails</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193dyvo</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>193d62n</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>about flaking/clouds nails</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193d62n</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>193cujo</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Why is the white of my nail so uneven? How can I make is more even?</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c94o6hnd7nbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>193dujx</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Gel Nails @ Home</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/193dujx/gel_nails_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>193c5d5</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Im so so proud of this set. Its inspired by the Starry Nights painting</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193c5d5</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>193dstz</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>I've spent years wondering what I'm doing so wrong with my nails</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193dstz</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>193b683</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Revived my natural nails!</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193b683</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>193akdd</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>How do you fix a thick French tip?</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/193akdd/how_do_you_fix_a_thick_french_tip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1939ybk</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>I can get gel tips and hard gel to stay on my nails for 3+ weeks, but BIAB always lifts within a day! What am I doing wrong? Is it just a bad gel?</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1939ybk/i_can_get_gel_tips_and_hard_gel_to_stay_on_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1937v4d</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Natural nails. No product.</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1937v4d</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1936qeb</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>Artists for inspiration</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1936qeb</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>193d819</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>I love this shade of pink! Just my favorite nails</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/plzk7dr4anbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>193czne</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>💖💖💖</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193czne</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>193bl1s</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Did a simple french on my own</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i3mjt1w0ymbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>193bj7w</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>My mom said they looked trashy...</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/46p9np5mxmbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>193bhrl</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>What would you pay for this fill in?</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ipboq2maxmbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>193b7vp</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>it’s nice outside. ☺️🥀✨</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pgeiafi8vmbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>193argw</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>I only started recently to use gel polish and I am so proud right now</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193argw</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>193ad8c</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Nails for my siblings baby gender reveal</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193ad8c</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>193abqc</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Rubber base and foil</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193abqc</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1939j7q</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Favorite set 😍</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ld65tfm0imbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1938s13</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>I haven’t painted my nails in forever. What colour would look best?</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/czkizb3nbmbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1938p70</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Just wanted to show this cute set I did for my friend's wedding</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1938p70</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1938igu</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Gel x, chrome, reflective glitter</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1938igu</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>19381b5</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>New Year, New Glitter ✨️</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19381b5</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1937pjr</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Swipe too see her glow up ☺️</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1937pjr</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1937ldh</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>Second rubber base manicure I ever did on my own nails</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fgmkad4p0mbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1937g2t</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>First set of the new year and I’m in love 💜</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wyi86ws8zlbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1933dni</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Difference between tapered square and square?</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1933dni/difference_between_tapered_square_and_square/</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>19369x4</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Buccellati Inspired Nails</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e1vq87owmlbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1936t44</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Best cuticle oil</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1936t44/best_cuticle_oil/</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1936fl0</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>Worth $0 and TV time?</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1936fl0</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1936bqe</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Always red</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tm10iv1hnlbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1935u5f</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>fake nails for narrow nail beds</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1935u5f/fake_nails_for_narrow_nail_beds/</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1935f2e</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Tips - polygel</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/epvzjaiyclbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>19357b7</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Any korean/ Asian normal polish brands?</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19357b7/any_korean_asian_normal_polish_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>193432q</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Gel-X Pink Daisy Nails!</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8clnopvcwkbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>193vken</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Digging the jelly</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193vken</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>193vir2</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Is the Orly Color Labs worth a visit?</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/diob2ok7erbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>193vc4j</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Super glossy dupes?</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0hhw2wg2crbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>193u2xt</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>feeling vintage 🤎</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wvbu3nvtyqbc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>193th8p</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Peel Off Base Coat Popping Off... Just... glue it back on?</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/193th8p/peel_off_base_coat_popping_off_just_glue_it_back/</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>193tevw</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>CND Shellac vs. Luxa Polish?</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/193tevw/cnd_shellac_vs_luxa_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>193td14</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Is ILNP Set Sail a good dupe for Cirque Sapphire?</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/193td14/is_ilnp_set_sail_a_good_dupe_for_cirque_sapphire/</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>193t9os</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Pink + holo space cowgirl set</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/19ohqpmoqqbc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>193sye3</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>tried glitter for the first time</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8bnkaqlrnqbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>193ssto</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Zoya - Dominique is so pretty. Pics don't do it justice.</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jn7itx6cmqbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>193sqet</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Really fell in love with this one...</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193sqet</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>193sorf</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>First magnet mani!</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tw4ccv19lqbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>193rsg8</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>My new favourite red!</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193rsg8</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>193rkjk</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>ILNP: Any stores in Las Vegas sell ILNP?</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/193rkjk/ilnp_any_stores_in_las_vegas_sell_ilnp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>193r8zs</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>Looking for colors similar to Nfu Oh 51 &amp; 52 (colored jelly base with shifting flakies and shimmer)</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/193r8zs/looking_for_colors_similar_to_nfu_oh_51_52/</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>193r7pr</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Simple and sparkly</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ywekpmgy7qbc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>193r13h</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Randomly stumbled on this combo, came out so pretty 😍</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193r13h</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>193pyl7</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Pop•arazzi from cvs</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193pyl7</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>193ptb6</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Proper QDTC usage</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fs8umyzvvpbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>193p120</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>My first Cirque Colors shade (Pixie Holo)!</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fa9olc0appbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>193p00j</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>my first magnetic polish!</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193p00j</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>193ozqz</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>ILNP - Sandy Baby</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193ozqz</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>193oyf0</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>A story in three parts</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193oyf0</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>193ogjh</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Black nails to match my mood</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zuoy3yflkpbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>193oci6</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Got my first magnetic polishes today 😊</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sfr8t9dpjpbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>193nw5n</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>glowyyyy</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kjdzifswfpbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>193nh1o</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Tips on removing stubborn gel polish (specifically at the ends)?</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r9in5uelcpbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>193na2z</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>A Mermaid Jelly Sandwich</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193na2z</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>193n6ny</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Cirque x Kelli Marissa 6 polish set is now $37.80 😱 (featuring Golden Nights new years nails)</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193n6ny</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>193n33s</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>I have no idea what I was going for but I kinda like it?</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/99aht3nm9pbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>193mzrh</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>🪴Monstera🪴</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193mzrh</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>193mmfz</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>What should I do?</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193mmfz</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>193mbsk</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Best bright pink with blue or purple shimmer?</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/193mbsk/best_bright_pink_with_blue_or_purple_shimmer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>193m0h8</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Portrait of a peach 🍑🖼</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/55shqdrd1pbc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>193l8y5</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>ILNP Magnetics! Which is your favorite?</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193l8y5</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>193kzdw</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Lyn B Designs sale on Friday Jan 12 2024</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/193kzdw/lyn_b_designs_sale_on_friday_jan_12_2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>193kqr1</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>My first-ever PPU polish - trying to will snow into existence</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193kqr1</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>193kiwr</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>SH Miracle Gel - One Shell Of A Party</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193kiwr</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>193jwyw</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>Magnetic heart with regular polish</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/s03hdse5mobc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>193j93d</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>What nail polishes are these?</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193j93d</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>193j3wn</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Time for valentines day manis already?? ❤️</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cimdps7bgobc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>193j3ro</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Trying out my new Sally Hansen Diamond Strength French Manicure Pen Kit</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193j3ro</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>193iy8k</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Nailtopia "Champagne Dreams" and Cirque Colors "Sun-Kissed" ✨️</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193iy8k</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>193ir2u</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Got a little (too?) creative.</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193ir2u</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>193iqiw</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>OBSESSED with this color + first time attempting a free-hand design</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0azwq3ggdobc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>193i4hv</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>One of my favorite noods</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193i4hv</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>193i438</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>ISO glowy topcoats</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/193i438/iso_glowy_topcoats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>193hvcg</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>I’m in love!</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ff9ydxgg7obc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>193hkuh</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Is this a top coat or a clear nail polish…?</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/193hkuh/is_this_a_top_coat_or_a_clear_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>193h2yj</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Madam Glam gel advice</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/193h2yj/madam_glam_gel_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>193gop6</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Trying to find this colour</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8mr23ngyynbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>193gm5z</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Orly Color Labs came out with Peach Fuzz to match Pantone's 2024 color of the year 🍑</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7epmxs1fynbc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>193gbgi</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Olive Ave Polish: Currant</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193gbgi</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>193fxqi</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Polishes I wore this week!</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193fxqi</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>193evpi</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Needed some summer vibes</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193evpi</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>193ektp</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>I saved a cat. The manicure paid the price</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193ektp</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>193efbc</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Frost Light</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ki4p3usinbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>193e1jd</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Obsessed with this blue glow</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8pw4fxh2gnbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>193dle1</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>do we like how jelly nails look on this length &amp; shape?</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193dle1</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>193bodx</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Every person deserves a best friend like mine</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5340urgoymbc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>193bnap</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Me: I’m not one of those high maintenance girls. Also me: *individually places sparkles on nails*</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/emq3lhhgymbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>193b29g</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>First tri-thermal polish!</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193b29g</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>193asdu</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>What I brought with me to my dorm</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193asdu</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>193aq8o</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I got my first thermal polish and I am OBSESSED </t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0ti8kpg0rmbc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>193ac85</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t xml:space="preserve">When the views are good but the nails are better </t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0bhdxitfombc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>193a9wu</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>wild berry west stole my 🩷</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193a9wu</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1937wdy</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>What drugstore polishes are good for stamping?</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1937wdy/what_drugstore_polishes_are_good_for_stamping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1935wfa</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Best monthly polish subscriptions?</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1935wfa/best_monthly_polish_subscriptions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>193417s</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>ILNP Sandbar visible nail after three coats</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193417s</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1933ywn</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>What nail polish do you always come back to?</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1933ywn/what_nail_polish_do_you_always_come_back_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1933gnn</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>POV: you’re wearing orly ‘won’t chip’ top coat 😔</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1lzo4z4kokbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>193wkfz</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Kawaii Chibi Mushrooms</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u1pawthrqrbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>193wi7b</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Blue China Nails</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193wi7b</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>193umch</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>French mermaid gel polish set</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k60cmdfe4rbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>193mps3</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>handmade wire art flowers! ♡</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/efeln6sr6pbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>193lxo2</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Portrait of a peach 🍑🤣</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1b5g5nbv0pbc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>193llmn</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Heart Nails ❤️🤍</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/saqu65acyobc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>193lccl</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>{ chichi nails in Ontario } metal chains styled art with 3D gel 🔩⛓️🪙🛠️⚙️ 💅</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i2l5tgohwobc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>193iem3</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Galaxy nails!</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193iem3</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>193i97b</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>it's like the wings of a butterfly 🥹🫶🏻</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3sbof3c7aobc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>193hs8i</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>Soft green mani set</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193hs8i</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>193dpfx</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Psycho but cute 👉🏻👈🏻</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193dpfx</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>193b6c3</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>My last work with stamping. Do u like design like this? 🥰</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0k2o8q3wumbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>193b3hp</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>My new work 🫦✨</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ok2os5yaumbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1939shw</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>It's on mermaid nails, isn't it? love my job 🥰</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1939shw</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1938l9j</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Love this set! Chrome !</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1938l9j</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1935oo2</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>My favorite nails from last month (⁠〃ﾟ⁠3ﾟ⁠〃⁠)</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1935oo2/my_favorite_nails_from_last_month_ﾟ3ﾟ/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Jan 12 08:08:09 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_01_14.xlsx
+++ b/data/2024_01_14.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C808"/>
+  <dimension ref="A1:C965"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14169,6 +14169,2675 @@
         </is>
       </c>
     </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>194pi61</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>These press ons from Etsy 😍💐</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194pi61</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>194ojfx</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>New year new nails</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194ojfx</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>194noe1</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>fresh set today (:</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194noe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>194nkqx</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Quick little blush almonds ⭐️</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fgrbbfvw5ybc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>194nh1l</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Gel Nail Lamp Annoyance</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/194nh1l/gel_nail_lamp_annoyance/</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>194m4si</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Moon &amp; star nails!✨</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194m4si</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>194lvr4</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>I know a lot of us are ready for V day nails BUT I have to show off this press on set I made ❄️🤍🎄</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194lvr4</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>194lq7i</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>simply in love with my nails🤍✨</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/11jafhcpnxbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>194lp92</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Cat eye</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t0fvzr9qnxbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>194lfpt</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Scissors or Bow Ties?</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s3s1z3a9lxbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>194ksre</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Playing with holographic nail polish</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194ksre</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>194iytl</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Wanted something neutral, nail tech suggest OPI Funny Bunny. I'm hooked...</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/56aa2vwazwbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>194io2u</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Fresh bday set</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qbmwi92twwbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>194iklz</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Simple set</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194iklz</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>194huzp</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Nail growing/strength tips?</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/194huzp/nail_growingstrength_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>194hpav</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Very happy with one hand and very unhappy with the other 😂</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194hpav</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>194hmd7</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>Simple pastel blush nail set design / purple cat eye</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194hmd7</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>194hlie</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>OPI ALPINE SNOW POWDER GEL W CHROME OVER TOP 🦄</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u7on7c81owbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>194hkkb</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Charge this customised size and design for 12 bucks yet the customer still haggled it down to 6 bucks</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o10vrihtnwbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>194hic7</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Charms and glue..</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/194hic7/charms_and_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>194hc3g</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>Press On Nails Newb</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194hc3g</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>194h3uj</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Met my nail tech in June, here’s my nails since ✨</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194h3uj</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>194h0h1</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>are my nails grown out enough to get an infill yet ?</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ib0s4ilajwbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>194gugk</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>New obsession: 3D gold Chrome tips</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5a0au9iyhwbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>194gu1n</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Matte Gel</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/194gu1n/matte_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>194gt0k</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Still practising 3d art, how did I do?</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194gt0k</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>194gjaa</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>6 months learning to do my own nails</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z5heecnjfwbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>194g0pg</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Bonding via nail painting with my teen daughter. Quality time and pretty nails. What more could a dad want?</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ilina2rlbwbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>194fyq1</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Moon nails</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194fyq1</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>194fdpi</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>A moment of silence please..</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jca0xgyv6wbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>194ehm1</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Trying to find brand/type of nail</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/194ehm1/trying_to_find_brandtype_of_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>194eca9</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>✨🪐 ✨</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194eca9</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>194e7dy</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>Nails I did for myself and my mom some time ago!! The long ones are my moms and the short ones are mine</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194e7dy</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>194dkpp</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Influence of UV nail lamps radiation on human keratinocytes viability - Scientific Reports</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.nature.com/articles/s41598-023-49814-7</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>194dhkg</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Hand sculpted/painted chocolate nails</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194dhkg</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>194d3wj</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Beauty and the Beast ❤️</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194d3wj</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>194cqmn</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Sparkly set ✨</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iqopzndknvbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>194cnst</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>Not sure about these!</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j63lpg00nvbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>194cm7o</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>January nail sets so far 💫 structured gel manicures on my client’s natural nails</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194cm7o</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>194c9x3</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Regrowing my paper thin nails</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/194c9x3/regrowing_my_paper_thin_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>194c8f9</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Gold “f you” accent nail</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u5wufu6tjvbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>194bnqg</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Gel Nail Polish to celebrate new job</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0uvznkbmfvbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>194bacr</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Set 1 of using up products I dislike!</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194bacr</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>194b9f3</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Mardi Gras Nails</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vre1922pcvbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>194b89t</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>A lot of work travel has made me disregard any previous love I had for my nails. Finally got a chance to get some pearly pinks again!</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iuz3ywqecvbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>194aw9r</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>I put my whole 🐱 into these!</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194aw9r</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>194a3pd</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>After 21 days, yesterday I finally chose something basic that goes with everything!</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1f5dkn244vbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1949yf0</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Did my own acrylic nails for the first time!</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1949yf0</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1949agz</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Yes, they really are my natural nails, this electric blue looks incredible</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ik2mgma2yubc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>19499lf</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Blue for January! ❄️</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19499lf</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>19497hm</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>What my nail tech did vs. what I showed her I wanted</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19497hm</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>19492bn</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Rubber Base Gel Recs (need help!)</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19492bn/rubber_base_gel_recs_need_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1948yid</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Nail art/</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z84pdvbovubc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1948rgv</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>I love it 💜</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1948rgv</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1948hmf</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>😍</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2feuspg8subc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1947kls</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Spring in winter 🥶</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1947kls</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1947erb</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Got a nail drill set for Christmas! Any advice is appreciated!</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z611xoehkubc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1947dfd</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>do you think that different nail shapes go better with different colors?</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1947dfd/do_you_think_that_different_nail_shapes_go_better/</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1947bnc</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Little shorter than I wanted but kept it simple with ombré</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xhghss6tjubc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>19477y1</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Press on sets that are missing doubles of some sizes.</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19477y1/press_on_sets_that_are_missing_doubles_of_some/</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1946oy2</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>💜</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cby1tp3efubc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1945qd4</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>DND/DC gel polish won’t cure</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1945qd4</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1945kde</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Builder gel over acrylic</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eiv4d5837ubc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>19456g8</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Kawaii Sanrio Press-on Custom ★</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19456g8</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>19443et</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Tried Flash-Reactive Polish</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2loh18xqvtbc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1943zwf</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>First set</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y09at4fwutbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1943gck</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>My natural nails haven't looked this nice in a while!</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0sgbw8kkqtbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1943g71</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>How to use a nail shiner</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1943g71/how_to_use_a_nail_shiner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>194329r</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>I was trying so hard to make it to 4 weeks and…</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kdpc12mfntbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1942cu3</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>My new pink babies 💅</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3f7m70wnhtbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1942afk</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Tried almond for the first time, with black chrome. What do we think?</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l95ol1z1htbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1941vi9</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>Amo!</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gm0uh6fgdtbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1941nwk</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>ROSE 😍</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/55fsa6ymbtbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1941g09</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Does my top coat need to be trashed</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i5t4msun9tbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>19415x2</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>Pressons that are actually short 🥰🌸🎀</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/i020o57u6tbc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1940m90</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>I got this colour and shape for the first time, how does it look?</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x5ln603r1tbc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>193z631</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>A good friend of mine just started doing nails and she did this amazing set🖤💛</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mjdnucolmsbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>193yiru</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>New set 🎀</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193yiru</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>193yckk</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Gel nails</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/193yckk/gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>193yc7m</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>One of my favourite manicure styles. So neat and simple and yet so lovely!</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dyvqm0kscsbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>193y328</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>How to Grow and Maintain Hyponychium?</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qzmigkdr9sbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>193w55m</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Help!!</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193w55m</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>193wekm</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Rounded sparkly stiletto nails</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m1lcdrdvorbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>193whgb</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>Not a nail tech but did these today</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ckhz7ubsprbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>193xkqk</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>polygel into biab??</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/193xkqk/polygel_into_biab/</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>193x84t</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>New nails for the new year ☺️</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193x84t</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>193x5kj</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>What can you say about such a manicure, this was the first time such a manicure was done, otherwise it always seemed to me that white gets smeared faster than others, but here with such a top it generally looks great</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dbi0gyivxrbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>194pn2u</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Garden Path Lacquers - I forgive you</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/t0esyzmksybc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>194otp0</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Lūmen Glass Jellyfish</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194otp0</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>194ocxe</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>Horseshoe Magnet Nail Hack</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194ocxe</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>194mqpm</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Strawberry fields 🍓 ✨</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194mqpm</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>194lncn</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>pink skittle</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194lncn</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>194kl1g</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Harlow &amp; Co - back in stock</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/194kl1g/harlow_co_back_in_stock/</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>194khri</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>A little color for a cold day</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194khri</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>194jpvv</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>Smokey Scream Ahead!</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194jpvv</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>194jnjd</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>I have found the perfect my nails but better formula!</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194jnjd</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>194jlv8</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Obsessed with this unexpected combo</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194jlv8</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>194iw0z</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>favorite nail polish brands?</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/194iw0z/favorite_nail_polish_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>194iqxf</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Cuticula is officially winning for my HG top/base coats because what the heck 😍</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vzvqc3ffxwbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>194i6k9</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>A godsend for polish removal</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dxvm4qarswbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>194hwey</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Blue hearts 💙</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194hwey</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>194hou7</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Had to brag about this $40 haul from a local store’s moving sale</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ghi813bsowbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>194hmfd</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Holo Taco Frost Light &amp; Scorched Earth</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8tii5jo8owbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>194gx9p</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Still hanging on for dear life :(</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k0ez2exkiwbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>194fo1i</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>First Beaux Reves Order!</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194fo1i</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>194ffd3</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Going with the teal trend</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5lt9tsi77wbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>194eyfc</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>Wanted some variety but this blue is so beautiful 😢 Gonna have to repaint the other three</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194eyfc</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>194ev55</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>my new hobby</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194ev55</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>194e8jf</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>This “evil eye” inspired design looks so cute with my new finger tattoos!!</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194e8jf</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>194e55e</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Shine bright like a diamond</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/riz35p1rxvbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>194dugq</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Nail Math: How I make $240 a year by painting my own nails</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ulk8kp4mvvbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>194dd6b</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>❄️🐆Snow Leopard🐆❄️</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194dd6b</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>194d844</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Tried The Magnet Trick- No Disappointment Here!</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/z7ww4sf5rvbc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>194d122</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Sorry for the aggressive claw video, but pictures don’t do ILNP’s Cameo justice.</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3fxd1khrpvbc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>194cwho</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Recommendations for warm-toned ILNP polishes?</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ttlbokctovbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>194c6jb</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Fallen Angels</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194c6jb</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>194bq3e</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Ruby Slippers vibes</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wvuol4z2gvbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>194bj5k</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Fresh and sparkly! 💚</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194bj5k</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>194bac8</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Fresh nails, got a chic manicure – feeling fabulous!</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gbraqufvcvbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>194adol</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Inspired by the winter storm outside</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ktrtj4m66vbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>194a0da</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>After the breakage of my middle finger nail (see last post) i glued a fake one on top and it works fine! Plus new maniqure</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wz44tzmu2vbc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1949q87</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>"we have mcdonald's at home" Macchiato Cloud dupe</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1949q87</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1949i2d</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Expectation vs. Reality - Cirque Colors "Fast Fashion"</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ifped4ylzubc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1949c8w</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Something icy with a little bit of warmth as we gear up for negative temps this weekend 🥶</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1949c8w</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>194956p</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>Was nostalgic for autumn today, I guess 🍂</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/79yxrmd0xubc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>194883r</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Trying to decide between a regular glitter gradient and a reverse glitter gradient</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/194883r/trying_to_decide_between_a_regular_glitter/</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1947x32</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Sad day for my mushroom nails 😞</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jiy1rx04oubc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1947lh8</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Aura nails with metal design 🫦</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nkjb6fgtlubc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1947fer</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Aura nails 🪄</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m09hoz5mkubc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1946fmd</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Cirque Colors - Snozzberry</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1946fmd</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1945mjc</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>First attempt at art on my third attempt at gel!</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rax5qblj7ubc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1945a28</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Three-color neutral holo mani</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1945a28</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>19442ac</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Open the door, get on the floor. Everybody walk the dinosaur 🦖</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qnqx87fhvtbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1943m7r</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>OPI - Squeaker of the House (on my little shorties)</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2yzzrv4yrtbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1943hvm</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>LA Colors - Believe In Magic 🤍</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1943hvm</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1943gep</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Finally went for a different colour</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/fPZCRJ5</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1942wwm</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>ILNP Eclipse versus Emily de Molly All The Rage</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/z75eapc7mtbc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1942pqd</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>obsessed with this color</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1942pqd</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1942l7m</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>I’ve recently been obsessed with magnetic polish. This is Cirque Colors “Blue Velvet”</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1942l7m</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>19424s2</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Elsa ❄️ ILNP</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19424s2</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>193zqp9</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Dots everywhere...</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193zqp9</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>194p9zf</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Nail tech in training, critique my work.(doing it for 2 months now, no I don’t charge full price)</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194p9zf</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>194nl7i</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Quick little blush almonds ⭐️</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r9ttw0316ybc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>194kd4j</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Design to add to bridal nails?</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/boro6w0abxbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>194gyvz</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Tried my hand at turquoise nails</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ap9kqcfuiwbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>194gi9a</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>my chrome nails: what am i doing wrong</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/omadwfmbfwbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>194ebv6</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>This “evil eye” inspired design looks so cute with my new finger tattoos!!</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194ebv6</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>194bsxb</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Would anyone like this Moroccan tile design?</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mimgdq3ngvbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>194bign</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Hello Kitty Inspired Acrylic Overlay</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cla3gzhkevbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>194a9dh</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Some clear pink nails by me ☺️</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eh6yko3a5vbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1948lh5</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Any criticism would be appreciated, i work full time but i really love nail art, this is technically my first attempt at full art, i paint and do alot of creative things anyway but id love to do press ons as a side hussle, on nail tips do i still need to apply polygel etc or is gel polish enough?</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u8su3fp0tubc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>19484e0</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>I did my own manicure and designed my nails 🥰</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19484e0</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>19448ew</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Reflective nails ✨✨✨</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lwkae88vwtbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1943q1f</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Loving the pink!!</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1o07nwjrstbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1942qif</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Probably my favorite set I’ve done</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sz7e227sktbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1941742</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>Pressons that are actually short 🥰🌸🎀</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rtd0qus47tbc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>193xm4m</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Too soon for Valentine’s Day nails?</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/193xm4m</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Jan 13 08:07:26 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_01_14.xlsx
+++ b/data/2024_01_14.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C965"/>
+  <dimension ref="A1:C1160"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16838,6 +16838,3321 @@
         </is>
       </c>
     </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>195iz1e</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>January 2024 nails</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ny1920psy5cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>195ij61</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Last set of 2023 idea was portals/portraits + galaxy</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/skfv72rnt5cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>195hrnn</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>I love love love the neutral colors with the acrylic sweater like lay over eeee. My favorite set I’ve seen so far 🤎🤍</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o4oq1i5qk5cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>195how2</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Valentines Nails… too chunky/low french tips?</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195how2</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>195hmbf</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Idk why I did this design but I like it somehow lol</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wk3ljzd4j5cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>195hgp8</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>I’m shy and experimenting with Gel X. Can you give me your honest thoughts?</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195hgp8</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>195hfb1</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>I have been a compulsive nail biter for as long as I can remember. I have decided to give up that habit. 3 weeks in!</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cfnsjt8sg5cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>195hc90</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Glue On Nails by Kiss — “Jelly Fantasy” … What do you guys think?</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195hc90</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>195guqh</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>I do my own nails at home and would like some constructive criticism please :)</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ssy2a12b5cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>195guir</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195guir</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>195ffap</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Do people notice if your nail polish isn't done perfectly?</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/195ffap/do_people_notice_if_your_nail_polish_isnt_done/</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>195fe7f</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Is there a glue I can use that doesn't last long?</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/195fe7f/is_there_a_glue_i_can_use_that_doesnt_last_long/</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>195fddc</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>What’s your favorite pink nail polish?</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/195fddc/whats_your_favorite_pink_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>195ex4d</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>OPI bubble bath + chrome</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195ex4d</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>195er5u</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Cute nails on fleek, ready to hit the road and conquer the day! 💅🚗</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bo3kk2cvp4cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>195eopr</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>“Frostbite” fresh acrylics!</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195eopr</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>195en2f</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>I’m obsessed with my January nails!!! They are so cute &lt;3</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195en2f</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>195ebal</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>just got my nails done. thoughts?</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195ebal</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>195e0cz</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>FRESH NAILS. What do you guys think? Does it suit me well?</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f8ccucejj4cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>195dwyo</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Second attempt using Builder gel</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0don81r0j4cc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1957mbc</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>What to do with peeling nails</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1957mbc/what_to_do_with_peeling_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>19583oa</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>How damaged are my nails?</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rk53wdat73cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1959i15</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Bone china</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fau76b1bi3cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>195dbhw</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>White Claws</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9yarmb9sd4cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>195dbfe</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Fun design for vacation</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/179qqagrd4cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>195arcy</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Help</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195arcy</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>195b72a</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>I need Valentine’s Day inspo!</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/195b72a/i_need_valentines_day_inspo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>195bwhr</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Definitely disappointed</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195bwhr</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>195cmv7</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>I Am What I Amethyst - OPI</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195cmv7</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>195cmcm</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Would anyone buy press ons like this?</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195cmcm</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>195cl13</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Don’t ask to see the dominant hand. Personal best, but still lots to learn</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195cl13</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>195ch5j</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>First DIY Dip</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195ch5j</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>195c3tc</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Nails before males! ;)</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/37d47yb634cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>195bog5</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>For a wedding next week</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x7zxosnpz3cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>195bg6c</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Freestyle, But Make It Intergalactic 👽</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195bg6c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>195beef</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>DIY nails</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/195beef/diy_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>195b7wf</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>freestyle set i did 🖤</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195b7wf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>195b6op</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>Structured gel manicure on her natural nails 🥹 Purple aura done with pigments x rose gold chrome 💜✨ (Her thumb nail and pointer nail on her dominant hand are short so she can pop her contacts in and out with no issues)</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195b6op</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>195armn</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Molto bellissimo 🥰</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wtcqjrp6s3cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>195aktf</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Cheetah Valentines Day Nails ❤️🐆</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qmuogfdoq3cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>195a2lh</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>New to doing nails … thoughts?</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195a2lh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1959t2e</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>These were not the easiest to do… how did I do?</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ynwc4ppqk3cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1959dkc</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Do I need an apex on short nails?</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1959dkc/do_i_need_an_apex_on_short_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1959c3b</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>My first time doing hybrid gel nails</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rzs3z9q2h3cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>19594k5</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Had beautiful coffin nails that barely lasted 2 weeks 😔 so disappointed. Not sure whether to chop the rest off or work with the 2 broken nails that I have.</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19594k5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1958r5y</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Practice pieces</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1958r5y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1958li9</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>What do you wish you'd known before you starting doing your own nails?</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1958li9/what_do_you_wish_youd_known_before_you_starting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1957omd</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Some of my favorite sets I got in 2023</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1957omd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1957lf6</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>$85 reasonable?</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dauhfzo143cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1957ay7</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>I love this gel polish🩵💙</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1957ay7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>19573ah</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>somewhat chaotic design</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jdwfmujb03cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1956x8y</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>-59⁰C with the windchill where I'm at, but at least my nails look cute🤭🥰</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9vr3ds21z2cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1956nc2</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Bug nails for my friend</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l0xmlg8xw2cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1956mbq</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Does this shape look good on my hand?</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b02aelapw2cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1956j4t</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Recent sets I’ve been working on</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1956j4t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1956hc2</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>I finally got to flip everyone off and get away with it</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1956hc2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1955t54</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Opalescence</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1955t54</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1955ip3</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Sou cute?</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9gw6fd9eo2cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1955hvd</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Hippie press ons I did at home</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9z41ypc7o2cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1954xeu</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Questions from the clueless.</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1954xeu/questions_from_the_clueless/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1954uzs</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Recent gel x sets I did on myself</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1954uzs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>19549lk</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Pearlescent topper?</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19549lk/pearlescent_topper/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1953x1q</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>More flexible gel x nails tips?</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1953x1q/more_flexible_gel_x_nails_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1953lsi</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>First time ever, would love to hear an opinion 🥲</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1953lsi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>19533im</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>Is this normal? Acrylic lifting near nailbed</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19533im</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1952qzl</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>Shiny black like my sole</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dadmz59v32cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>195233l</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>Re-did my nails and love them this time!!</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195233l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1951vy9</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>First time trying stickers</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1951vy9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1950h52</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>It's hard to capture the holo effect</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6vugeeq0n1cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1950fmr</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>Brittle nails - gel manicure?</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1950fmr/brittle_nails_gel_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>194zmp2</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Glitter 😍</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194zmp2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>194zm8w</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Just done, in love with them</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wt4ckbwsg1cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>194wop8</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>DIY BIAB nails 💅</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194wop8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>194suti</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Eras Tour Nails</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/194suti/eras_tour_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>194zedt</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Wanted to share some of the nails I did on myself over the years</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194zedt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>194rqwr</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>Help!! Can anyone tell me why my topcoat goes matte at the tops of my nails?</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ajbx57cizbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>194rp33</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>I put on fake nails but I could never get the cuticle area to look good. What can I do to improve it?</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194rp33</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>194okf3</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Progress! I'm not perfect, but I'm happy I stuck with this hobby ♥️</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194okf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>194z5so</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>I'm in love 😍</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rm3gersdd1cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>194kp4n</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Still learning how to do these but here’s my attempt at some valentines nails</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p3l4y6n9exbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>194z2uw</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>:)</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194z2uw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>194yvr5</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Removing putty from nails</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/194yvr5/removing_putty_from_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>194gshb</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>i paint my own natural nails, why does my matt gel top coat get weird and wrinkly??</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194gshb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>194gdni</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>my chrome nails: what am i doing wrong</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xfoqysbbewbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>194g630</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>Thoughts on Dazzle Dry?</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/194g630/thoughts_on_dazzle_dry/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>194ykrt</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>My happy lil dopamine nails</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194ykrt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>194e73b</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Watermelon nails I got two days ago to celebrate summer</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8w5qvy75yvbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>194c1d5</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>I love how cute this evil eye inspired design looks with my new finger tattoos!</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194c1d5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>194b8gx</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>This is probably the best set I’ve done on my husband 😮‍💨</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194b8gx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>194aacl</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>just some inspo from my fav set ive gotten, is it weird to get again in diff color?</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194aacl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>194y847</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>how can i maintain the growth?</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bs5hb66861cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>194y6rd</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>New gel nails💅🏼 what do you think?</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uvekzmox51cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>194xlw6</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>Ditched the nail technician 💅🏻</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194xlw6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>194x6vi</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>January and December the toes xan catch up.</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ga0dq4eay0cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>194wuhj</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>First Gel Mani... are they supposed to look like this?</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/194wuhj/first_gel_mani_are_they_supposed_to_look_like_this/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>194vwqb</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Does anyone else get nails that look good with a tan!? Isn’t this blue so pretty and simple!!</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hg8qqozzn0cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>194v9db</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Eye can see you👁</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194v9db</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>194v10c</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Can I use regular nail glue to softgel nails?</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/194v10c/can_i_use_regular_nail_glue_to_softgel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>194uoxc</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>A different take on glowy blue 🦋</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194uoxc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>194um7p</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Used builder gel for the first time.</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194um7p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>195hydj</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Spotted Cort</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195hydj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>195gdsg</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Dream within a Dream</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195gdsg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>195g6jl</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>I finished! Step one of my master plan is complete.</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195g6jl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>195fut3</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>At least my nails match the weather</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gxyz0zay05cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>195fml9</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Shimmery reddish brown/brownish red</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195fml9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>195fkad</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>absolutely obsessed with this glow ✨</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195fkad</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>195febx</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Flakies dupes?</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195febx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>195ed03</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Nail color Cirque Georgette</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7z2oeih2n4cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>195dsx5</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Anniversary nails</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mcdnnjn1i4cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>195defr</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Thinner in QDTC</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/195defr/thinner_in_qdtc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>195cysn</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>A fresh filing feels so good! Finally got my hands on Macchiato Cloud 🌧️</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oi9wb1vna4cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>195cq2h</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>Lyn B</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/195cq2h/lyn_b/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>195c3m4</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>What do you guys/gals think of me as a straight guy getting my nails done(feeling pretty self conscious)</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pv0a293b34cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>195bhob</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>Wow what a surprise! What range!</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195bhob</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>195akii</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Nail polish purge advice</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/195akii/nail_polish_purge_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>195ak0k</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>The perfect polish for an aquarium trip 🐟</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zjteojxhq3cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>195a253</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Limerance 💚✨DVN</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/k7t9564lm3cc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1959fx3</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Top Coat recommendation for KBShimmer Glitters?</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5p7ml3tvh3cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>19597x0</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Feeling spacey 🛸👽</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19597x0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1958z2x</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>It's been SO Satisfying swatching all my polishes! But...this is only half. I have a problem.</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/Kh0CyZV.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1958ec4</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>My favorite slimy green</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0pagmg71a3cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>195764h</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Addiction</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xasrp9kv03cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>19573gn</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>My signature mani is definitely dark red half moons, what’s yours?</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19573gn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1956rc6</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>I love it when a plan comes together 😍💜</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6y6b4idrx2cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1956h4e</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Zoya Bijoux is so soft and feminine with lots of holo sparkle!</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tfmu4bzkv2cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1956gt6</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>Reckless</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ixmgy7div2cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1956f0f</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Love jelly polishes!</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7xzwsgn4v2cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>195675a</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Can chrome be used with normal nail polish top coat?</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/195675a/can_chrome_be_used_with_normal_nail_polish_top/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1955z1l</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Magnetics 😍</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1955z1l/magnetics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1955nkq</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Snowy January look ❄️</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1955nkq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1955ggr</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>I’m a January baby, so it was time to bust out Garnet 💎❤️</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1955ggr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1955d4o</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Crystal Knockout Formula?</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://hellahandmadecreations.com/collections/hhc-january-14th-21st-2024-monthly-releases/products/crystal-knockout-dragon-princess-capped-pre-order</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>19550a0</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>I recived practice finger as gift and I need some insight</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mld24x2kk2cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1954abf</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Pearlescent topper?</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1954abf/pearlescent_topper/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1953uym</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>As BRIGHT as lava 🔆🌋 🔆</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1953uym</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1953ke9</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Velvet Magnetic Jelly Sandwich🎀</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/r2ay104u92cc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1952ylb</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>Advice on Shape</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1952ylb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1952y43</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>ILNP Emma 💙</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1952y43</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1952ox6</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Renos broke them all bur still tried water marbling 1st time</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1952ox6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1952jrr</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>His Gentle Ruler</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4q5zbujc22cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1952gy9</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>The Blue Dragon</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1952gy9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1952gxl</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Trippy black light nails!</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1952gxl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1952arz</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Mystery from LynB or Emily de Molly?</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1952arz/mystery_from_lynb_or_emily_de_molly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>19526ps</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>Not cool man...</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19526ps</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1951xea</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>Received some lemmings and re-added some old favorites to my China Glaze collection! Shade names will be in the comments</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jewowxhpx1cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1951tdx</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>Snow day in Illinois</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1951tdx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1951r0m</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Besides Harlow and Co where can a Canadian order A England from?</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1951r0m/besides_harlow_and_co_where_can_a_canadian_order/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1951i18</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>album-inspired nails ✨️</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1951i18</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1950ye3</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>First mani of 2024! 😊</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1950ye3/first_mani_of_2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1950yc0</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Icy Blue</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1950yc0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1950udi</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Granite nails</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5d406yqpp1cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1950r85</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Are these cute or are they too busy? Should I redo them with just two colors?</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mo4w63j1p1cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>195034i</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>nail polish came off one finger at work and i was tired of looking at my bare nail in my peripheral vision</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195034i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>195031l</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>My prugly heart is singing! OPI's Who The Shrek Are You? is a perfect color match to Shrek's skintone</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eq9glbtoj1cc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>194zpmd</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>Jelly Nails</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/194zpmd/jelly_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>194zi3c</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Nail Journey - 4 months 😊</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194zi3c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>194uqkv</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>I decided to finally join team BIAB. I think the results speak for themselves.</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7sdtem94e0cc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>194zfha</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Guess I'll shop Hellahandmade this month, what's on your wishlist?</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ncifwbff1cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>194z2e1</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Holy shift!</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194z2e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>194z1c6</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Nourishing Nude by Orly Breathable 😍</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194z1c6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>194ypaw</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>Feeling Katniss Everdeen Girl on Fire</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194ypaw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>194yj8w</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Snow Day Manicure</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ti9agtnj81cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>194d4s7</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>Mooncat Vaporize Dupe</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/194d4s7/mooncat_vaporize_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>194b3dz</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Layering top coats</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4klyhvjgbvbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>194a2tu</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>I just got my Zoya 10 for $25 order ☺️ I had to try this one right away! Polishes Used: Zoya (Shade: Bisoux) | Seche Vite (Gel Effect Top Coat)</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194a2tu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>194xwhh</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>{Gifted} Blue Velvet by Cirque Colors 💙</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y5uj39bn31cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>194xpas</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>Matched my mani to the moody music I’ve been listening to lately</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b1yk6fo621cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>194xbjm</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Splurged on adorable nail art</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194xbjm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>194x7a8</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>Zoya Polaris would make a beautiful wedding polish</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fqt471mdy0cc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>194vqck</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First ever attempt with magnetics and I’m obsessed! </t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kra7jr1mm0cc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>194v3br</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>Night sky nails 🌌</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194v3br</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>194v23j</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Please join me in mourning this loss 😫</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b0cxqzrxg0cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>194ugau</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Chipped nail help</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ajvl9tmb0cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>194u5w3</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>It looked disappointing in the bottle but I fell in love when I put it on 😍</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n2io03ev80cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>194qmfn</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>January flames 🔥</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6tkkdq0k4zbc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>195drlx</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Eras Tour Nail Inspo</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/195drlx/eras_tour_nail_inspo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>195cte9</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Beginner and unsure what to do!</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/195cte9/beginner_and_unsure_what_to_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>195bi5j</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Space Vibes 👽</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195bi5j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>195bht2</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Harry Potter nails I did on my client today!</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195bht2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>195axdt</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>Practice sheets?</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/195axdt/practice_sheets/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>195alr6</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>Cheetah Valentines Day Heart Nails 🐆❤️</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wq937vcwq3cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>19589ws</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>Addicted to the holo powder 😍</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a4oh7i4493cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>19571t4</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>Some Burberry Inspired Nails</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t79wr9k003cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1956r5r</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Fire🔥</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gu1n0xppx2cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1956g7k</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>Recent sets I’ve made</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1956g7k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>19545l1</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Simple but fun!</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19545l1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>195307m</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>where to buy charms online?</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/195307m/where_to_buy_charms_online/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>19515iy</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Missing these from Halloween 🥲</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19515iy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1950bww</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Practice using solid builder gel</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m1vme6hxl1cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>194zaz6</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>Nail Art on Gel-X</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194zaz6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>194yt5u</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>Fresh set 💅🏼💚💙</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194yt5u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>194xgfi</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>Barbie nails 🎀</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/194xgfi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>194ufgm</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>Practice set, inspired by my nostalgia of arcade carpets.</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2qy998udb0cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>194tgq2</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>Black Lace + roses</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ea426enp10cc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>194q509</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>Aura nails 🪄</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uwrtztafyybc1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Jan 14 08:07:19 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_01_14.xlsx
+++ b/data/2024_01_14.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1160"/>
+  <dimension ref="A1:C1328"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20153,6 +20153,2862 @@
         </is>
       </c>
     </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>196axw2</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>nail art done by my sister ❤️❤️</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gdk9jinc5dcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>196ajnc</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Do these ok? Went out of my comfort zone.</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/196ajnc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1969bhq</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>Week old BIAB but I am so pleased with their simplicity and elegance I wanted to share them, thoughts …..</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u3ow9lywmccc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1968jfp</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>first attempt on french tip + blooming gel</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1968jfp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1968io3</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>First time getting acrylics done 💋</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1968io3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1968ae6</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>fresh manicure</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1968ae6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1967p0m</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>I always bling my nails</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/byk88lt36ccc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1967ekq</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Longest you’ve had an acrylic set on before getting a completely new set?</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1967ekq/longest_youve_had_an_acrylic_set_on_before/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1967ce0</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>Im so proud of myself</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1967ce0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1966pni</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>Sweater nails I did on my coworker</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1966pni</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>195xpgg</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>what I got (@nailsbysandyyy) vs the inspiration (@mjnailz)</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195xpgg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1966an7</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>How Much Do Acrylics Typical Cost</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1966an7/how_much_do_acrylics_typical_cost/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1962ia0</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>What I asked for vs what I got 😊</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1962ia0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1963o74</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>why does the gel peel off easily</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1963o74/why_does_the_gel_peel_off_easily/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>19665ns</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>Which lasts longer gel/shellac or gel nail strips? Which one is better?</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19665ns/which_lasts_longer_gelshellac_or_gel_nail_strips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>196600g</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>Dark colours on pale hands</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/my8qvyuepbcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1965ome</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Determined to post all my nails from my nails journey!</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1965ome</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1965o8k</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>I normally don’t do bold colors but I’m obsessed!</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a74qrtmfmbcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1965evk</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>These are my natural nails, index just broke. Should I cut them all?</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vhttyk6zjbcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1965dy2</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>I just picked the colors and gave her and gave her a gothic theme and she killed it!</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/264huitqjbcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1965ale</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>First time ever doing my own nails and I have a lot to learn but pretty pleased</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1965ale</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1964xfc</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>I HAVE FINALLY FOUND MY DREAM NAIL TECH</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1964xfc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1964ono</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>First time trying polka dots on daughters nails</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1964ono</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1963rom</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>I need top coat suggestions</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1963rom</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1963jq3</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>I know they’re a lot but I’m so happy</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1963jq3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1963fhq</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>nails check 💅🏻 🎀</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s05gkmh32bcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>196304s</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>Something a little different</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iyz9th1pyacc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1962uua</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>My first glitter powder set</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fytyky1gxacc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1962956</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Can I get your feedback please?</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1962956</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>19627ck</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>BIAB Nails Help !</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oz7ddgfxracc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1961ypf</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Louboutin nails</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1961ypf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1961ubx</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Back to the Dazzle Dry!</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/agqw4c3woacc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1960z5w</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>Halp? Removing gel polish</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1960z5w/halp_removing_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1960chy</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Need advice! I just got my nails done today. I was eating popcorn and now my pointer fingernail is stained yellow from the salt and butter. I tried scrubbing it off with dishsoap and it didn’t do much. Is there anything I can do to fix this?</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i9grz60ncacc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1960br1</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>Gel x set</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1960br1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>196053w</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>Pink and white glitter nails!</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v7lnnniyaacc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>195zv1c</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>First attempt at sweater nails</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9f5elb8q8acc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>195zug3</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Peacock nails</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195zug3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>195zu9v</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Absolutely love this design 💜</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195zu9v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>195zohl</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>I just got almond nails, which shape looks best on me? I seriously can’t decide, haha</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195zohl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>195zdaq</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>First Set of 2024!</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195zdaq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>195yyie</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>butterflies n glitter 🦋🩵✨</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kts9oc1n1acc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>195yrgc</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>New Set !</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3i8zw2530acc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>195yloy</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>Did my own gel set (and first matte set) for the first time! Thoughts on shape or any tips?</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195yloy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>195yixl</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>Addicted to the holo powder 💕</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y2h5txq5y9cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>195ye14</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Trying nail art again after 11 year hiatus</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195ye14</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>195y76h</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Y'all Motivated Me!</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rvx95vqlv9cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>195y6xa</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>First manicure of the year</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195y6xa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>195y41k</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Let me nails deteriorate for a while, feels good to paint them again</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6jbd9o0xu9cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>195t1jq</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>How do I cap the free edge on very tiny and thin nails?</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195t1jq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>195xtz3</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>Tried a new salon yesterday, expensive but really happy with them!</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/84kk2kdrs9cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>195xmgo</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>💙🩶 ILNP Overcast Collection ☔🩵 (minus Daybreak)</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195xmgo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>195xlaf</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>Winter nails</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0bhbujurq9cc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>195xg6c</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>Guess who the bride is</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t2ydyiipp9cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>195whh6</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>Is it normal to have a few bubbles and polish crusties on the sides of your nails after getting them done or am I just being picky?</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nx20sutbi9cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>195wchy</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>Struggling to get poly gel off</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195wchy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>195w7md</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>I'm obsessed with that thermal nail polish</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195w7md</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>195vyr1</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Don't know what to call these but I'm in love! </t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8scp14p8e9cc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>195v88y</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>Press On Nails</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/195v88y/press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>195ux9s</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>Finally found my perfect pinkish nude nail color</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/195ux9s/finally_found_my_perfect_pinkish_nude_nail_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>195uw19</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>Additional Pics: Home Gel French</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195uw19</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>195ure2</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>New Nails</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w2hpyu1359cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>195ulp7</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>Home gel French</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nr5l5jwu39cc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>195tvci</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>Cuticle oils</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jk8u2deay8cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>195tv2l</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>Sacrifice to the snow gods</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/areuab18y8cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>195tpot</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>Floral gel strips! 🌸🌻🥀💐</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195tpot</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>195tokw</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>Being a nail girly and requests rant</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/195tokw/being_a_nail_girly_and_requests_rant/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>195tix7</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>I love these Blue glitter</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195tix7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>195tdzi</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>A creamy, matte nude</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7xzeh0biu8cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>195t8r4</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>Black and gold nails</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195t8r4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>195t48r</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>Loving my new nails, but I feel like I definitely got overcharged 🙂</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k3zia2bes8cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>195t2xl</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>New press on set I did! Opinions?</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195t2xl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>195syi2</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Length? Shape?</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m3z2b715r8cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>195sg0k</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>I think the most beautiful thing are the stones that I put on my nails✨</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ocrbbzt3n8cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>195khrd</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>how do i improve?</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195khrd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>195g6id</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>Where to buy velvet cat eye gel? Photo from @akina_enoi from Instagram. The gel is the photo is from enoi.</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sei9477745cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>195g6bk</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>Gel-X square tips keep breaking?</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/195g6bk/gelx_square_tips_keep_breaking/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>195rmyn</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>The colour of my nails match my drink perfectly! On another note this polish is so much cuter than I thought it'd be.</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/co4lq1trg8cc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>195rhpi</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>Which nail shape suits my hands better? (Almond/Coffin)</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195rhpi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>195qyr5</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>Butterfly wings 🦋</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195qyr5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>195qxlo</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>Did my nails with Gel for the first time in 2 years 🤍 really missed it</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195qxlo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>195qclr</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>First attempt at using nail stickers</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vb4z802l68cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>195pwcu</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>First time doing gel extensions!</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qercacls28cc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>195p32r</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>DIY extension for the first time</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195p32r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>195ny7n</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>Just started doing my own nails</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/odtfljz9l7cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>195niwf</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>Need advice</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/195niwf/need_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>195lih9</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>First set of the year, I'm in love ❤️</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195lih9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>195jp2m</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>Learning to do my own nails</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bgcwbh3m76cc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>195jixq</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>Press on nails or semi cured gel strips?</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/195jixq/press_on_nails_or_semi_cured_gel_strips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>195jf3m</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>A Lovely Night</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195jf3m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>196ajn1</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>my new obsession</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dfej9i1n0dcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>196a4sy</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>ILNP la Catedral</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xlu4cd10wccc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1969yiv</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>Full Scream Ahead</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1969yiv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1969hfk</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>My first experience with ILNP was mega</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qs3xypfpoccc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1969clr</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>Everyone is prepping for a winter freeze in Texas. I'm prepping winter nails. I have my priorities in order. 🥶❄️</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1969clr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1968eim</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>Went for mismatched nails this time</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1968eim</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>19689vi</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>Double topcoat question</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19689vi/double_topcoat_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1967voi</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>Did those cute little coffee themed nails</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1967voi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1967nxe</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>Guess I'm taking a break from swatching</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qoi45wlr5ccc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1967js0</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>This color is way prettier than I expected</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1967js0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1967cnl</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>Snow Day Mani</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1967cnl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1966una</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>Rejuvacote nail growth system</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1966una/rejuvacote_nail_growth_system/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1966h6j</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>Label Maker recommendation for nail swatch sticks?</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1966h6j/label_maker_recommendation_for_nail_swatch_sticks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>19660kd</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>Second mani of the year,</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rxn0z6wjpbcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>196521k</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>Zoya - Kira</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/302p0pkpgbcc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1964tja</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Yep... it was a good choice.</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1964tja</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>19625j3</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>I love this brown satiny polish, but…</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19625j3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1961wrb</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>Are you yeti for snow?</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1961wrb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1961bs9</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>“Winter” but make it fun</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1961bs9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1961ayd</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>I love berry jellies</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ibj8ih1ekacc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>196107y</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>What's your favorite magnetic polish?</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mkleo1vxhacc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1960uji</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>Overstuffed stamping with mixed mattes.</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1960uji</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1960sfr</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>INM Fast Drying Top Coat vs INM Northern Lights Holographic Top Coat?</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1960sfr/inm_fast_drying_top_coat_vs_inm_northern_lights/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1960rft</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>One manicure to rule them all.</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1960rft</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>195zl4c</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>Cirque jelly gradient 🩷💜🩵</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195zl4c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>195ynu9</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>Vitamin D🌞</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195ynu9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>195yfpu</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>Checkerboard Nails!</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195yfpu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>195xxjn</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>Found a polish to match my hoodie. Figured y’all would understand.</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195xxjn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>195xsid</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>Moonstone</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yprqv9ffs9cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>195xmih</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>Bees Knees Lacquer Splurge</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ne3h2xy2r9cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>195xlje</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>💙🩶 ILNP Overcast Collection ☔🩵 (minus Daybreak)</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195xlje</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>195xdws</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>Not a fresh mani but it’s holding up so well!</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195xdws</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>195wxz1</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>What time are Lumen releases?</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/195wxz1/what_time_are_lumen_releases/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>195ws10</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>indie / boutique nail brands sales data?</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/195ws10/indie_boutique_nail_brands_sales_data/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>195w4n8</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>Bridal nails - can I have fun?</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/195w4n8/bridal_nails_can_i_have_fun/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>195vrt0</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>Dusky Mood with Zoya Neeka</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lg4nv5ftc9cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>195vo08</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>Painted my nails after almost a year</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1qrlk4c0c9cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>195vlxj</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>AHHHH!</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195vlxj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>195vlv0</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>Trends for 2024</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j6x1lt7kb9cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>195vkgm</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>Glowey Grunge</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195vkgm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>195vca9</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Swatch: Late Checkout</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195vca9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>195v07k</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>You’re A Twat — Swamp Gloss</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195v07k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>195upf3</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>How do I make my White/ Clear Nails look better?</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gmvbjqgn49cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>195ude5</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>Cozy vibes</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u4zmtoa329cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>195ucxb</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>Non stamping polishes recommendations</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195ucxb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>195tha1</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>Builder gel polish hurts when curing?</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/195tha1/builder_gel_polish_hurts_when_curing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>195svs5</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>Trying to shop my collection more often</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j9utr34jq8cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>195svaw</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>Similar Polishes?</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o862vbsfq8cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>195stu3</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>Fairy Dust 💜</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195stu3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>195stnm</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>Why does ethereal polish have such a cult following?</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/195stnm/why_does_ethereal_polish_have_such_a_cult/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>195sqzh</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>MOTN + Silver Flake Taco</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5rbpdnbfp8cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>195sppv</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>Zoya sale for the win</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195sppv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>195siv7</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>Sprinkle</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195siv7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>195s2kp</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>Feeling blue today!</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nycmiax6k8cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>195ruq4</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>Finished swatching and organizing my glitter collection</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m4u2is9hi8cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>195m16f</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>What better way to try out my Zoya haul than a skittle? 🩷💜💙 Polishes Used (Pinkie to Thumb): Zoya (Shade: Malana) | Zoya (Shade: Aurora) | Zoya (Shade: Kira) | Zoya (Shade: Inez) | Zoya (Shade: Tamiah) | Seche Vite (Gel Effect Top Coat)</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195m16f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>195r63s</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>💜🍌Bananas🍌💜</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195r63s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>195qpuh</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>Help me Find!</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/98qw4dsk98cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>195qmik</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>Ammolite skittle!</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kfkrcunu88cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>195q3iy</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>First Time Using Nail Stickers.</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ukmqw86h48cc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>195pet8</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>I feel like the shade looks nicer on me IRL</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dnouf4fqy7cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>195or3f</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>Cuticle buddy scents</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/195or3f/cuticle_buddy_scents/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>195ob7e</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>What can I expect at PBE?</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/195ob7e/what_can_i_expect_at_pbe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>195lb8w</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>Too broke to buy the dress, wearing ILNP's Olive Grove instead</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jgripnd1s6cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>195ju36</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>Accidental nail x outfit coordination 😌</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195ju36</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1969xyq</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>Todays sets!</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1969xyq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1967qna</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>Pink or purple ?</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1967qna</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1967aky</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>Winter nails I made</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/15q9dfxy1ccc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1965hoi</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>Ready for the game tomorrow 💙🦁</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qzyg6d1rkbcc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>19612ic</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>Overlay on natural nails.</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jl38228hiacc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>195z4nm</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>Te las harías?</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/04fobucz2acc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>195wqpv</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>New acrylics</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195wqpv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>195w6y5</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>Icy nails</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1jpuc1f2g9cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>195vy97</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I don't know what to call these but I'm in love! </t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hcjylah5e9cc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>195vf30</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>Headed to Miami for my birthday, and my girl @nailedtothecounter set me up right.</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xdl4aq74a9cc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>195s7xy</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>Got them artsy lesbian nails lol</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195s7xy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>195nng6</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hand painted hibiscus flowers 🌺 </t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yv3v9aiai7cc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>195n30t</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>My first set of the year. Barbie vibes or early valentines vibes because of the heart?</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/195n30t</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>